<commit_message>
Final chart for presentation - Apps by Genre.
</commit_message>
<xml_diff>
--- a/queries_for_presentation/top _100_by_genre_with-roi-and-more.xlsx
+++ b/queries_for_presentation/top _100_by_genre_with-roi-and-more.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,24 +8,34 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lorib\Desktop\NSS_Data_Analytics\projects\app-trader-kiwi\queries_for_presentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{B4693B2E-E29D-4828-8EFE-1C48A883BD85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64584F89-A8C8-4C9C-881A-EBA8BC8CFE86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="2340" windowWidth="22815" windowHeight="13110"/>
+    <workbookView xWindow="840" yWindow="1065" windowWidth="17310" windowHeight="14055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FINAL CHART" sheetId="2" r:id="rId1"/>
     <sheet name="top _100_by_genre_with-roi-and-" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'FINAL CHART'!$A$1:$C$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'FINAL CHART'!$A$1:$E$14</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'top _100_by_genre_with-roi-and-'!$A$1:$I$14</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
   <si>
     <t>genre</t>
   </si>
@@ -99,28 +109,64 @@
     <t>Genre</t>
   </si>
   <si>
-    <t>BOOKS &amp; REFERENCE</t>
-  </si>
-  <si>
-    <t>FOOD &amp; DRINK</t>
-  </si>
-  <si>
-    <t>NEWS &amp; MAGAZINES</t>
-  </si>
-  <si>
     <t>Average Profit</t>
+  </si>
+  <si>
+    <t>SPORTS (4)</t>
+  </si>
+  <si>
+    <t>FINANCE (3)</t>
+  </si>
+  <si>
+    <t>BOOKS &amp; REFERENCE (2)</t>
+  </si>
+  <si>
+    <t>EDUCATION (2)</t>
+  </si>
+  <si>
+    <t>PHOTOGRAPHY (1)</t>
+  </si>
+  <si>
+    <t>COMMUNICATION (1)</t>
+  </si>
+  <si>
+    <t>PRODUCTIVITY (1)</t>
+  </si>
+  <si>
+    <t>FAMILY (26)</t>
+  </si>
+  <si>
+    <t>GAME (53)</t>
+  </si>
+  <si>
+    <t>FOOD &amp; DRINK (2)</t>
+  </si>
+  <si>
+    <t>SHOPPING (2)</t>
+  </si>
+  <si>
+    <t>NEWS &amp; MAGAZINES (1)</t>
+  </si>
+  <si>
+    <t>LIFESTYLE (2)</t>
+  </si>
+  <si>
+    <t>Genre - App store actually SUB-GENRE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Used CATEGORY in </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -607,12 +653,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="21" builtinId="30" customBuiltin="1"/>
@@ -768,7 +815,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'FINAL CHART'!$B$1</c:f>
+              <c:f>'FINAL CHART'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -793,58 +840,58 @@
               <c:strCache>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>SPORTS</c:v>
+                  <c:v>GAME (53)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>FINANCE</c:v>
+                  <c:v>FAMILY (26)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>BOOKS &amp; REFERENCE</c:v>
+                  <c:v>SPORTS (4)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>EDUCATION</c:v>
+                  <c:v>FINANCE (3)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>PHOTOGRAPHY</c:v>
+                  <c:v>BOOKS &amp; REFERENCE (2)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>COMMUNICATION</c:v>
+                  <c:v>EDUCATION (2)</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>PRODUCTIVITY</c:v>
+                  <c:v>PHOTOGRAPHY (1)</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>FAMILY</c:v>
+                  <c:v>COMMUNICATION (1)</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>GAME</c:v>
+                  <c:v>PRODUCTIVITY (1)</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>FOOD &amp; DRINK</c:v>
+                  <c:v>FOOD &amp; DRINK (2)</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>SHOPPING</c:v>
+                  <c:v>SHOPPING (2)</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>NEWS &amp; MAGAZINES</c:v>
+                  <c:v>NEWS &amp; MAGAZINES (1)</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>LIFESTYLE</c:v>
+                  <c:v>LIFESTYLE (2)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'FINAL CHART'!$B$2:$B$14</c:f>
+              <c:f>'FINAL CHART'!$D$2:$D$14</c:f>
               <c:numCache>
                 <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>1060000</c:v>
+                  <c:v>1062530.19</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1060000</c:v>
+                  <c:v>1066000</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1060000</c:v>
@@ -862,10 +909,10 @@
                   <c:v>1060000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1066000</c:v>
+                  <c:v>1060000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1062530.19</c:v>
+                  <c:v>1060000</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>1084000</c:v>
@@ -908,7 +955,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'FINAL CHART'!$C$1</c:f>
+              <c:f>'FINAL CHART'!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1104,58 +1151,58 @@
               <c:strCache>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>SPORTS</c:v>
+                  <c:v>GAME (53)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>FINANCE</c:v>
+                  <c:v>FAMILY (26)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>BOOKS &amp; REFERENCE</c:v>
+                  <c:v>SPORTS (4)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>EDUCATION</c:v>
+                  <c:v>FINANCE (3)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>PHOTOGRAPHY</c:v>
+                  <c:v>BOOKS &amp; REFERENCE (2)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>COMMUNICATION</c:v>
+                  <c:v>EDUCATION (2)</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>PRODUCTIVITY</c:v>
+                  <c:v>PHOTOGRAPHY (1)</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>FAMILY</c:v>
+                  <c:v>COMMUNICATION (1)</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>GAME</c:v>
+                  <c:v>PRODUCTIVITY (1)</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>FOOD &amp; DRINK</c:v>
+                  <c:v>FOOD &amp; DRINK (2)</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>SHOPPING</c:v>
+                  <c:v>SHOPPING (2)</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>NEWS &amp; MAGAZINES</c:v>
+                  <c:v>NEWS &amp; MAGAZINES (1)</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>LIFESTYLE</c:v>
+                  <c:v>LIFESTYLE (2)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'FINAL CHART'!$C$2:$C$14</c:f>
+              <c:f>'FINAL CHART'!$E$2:$E$14</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>757.14</c:v>
+                  <c:v>754.59</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>757.14</c:v>
+                  <c:v>756.49</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>757.14</c:v>
@@ -1173,10 +1220,10 @@
                   <c:v>757.14</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>756.49</c:v>
+                  <c:v>757.14</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>754.59</c:v>
+                  <c:v>757.14</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>743.05</c:v>
@@ -1258,6 +1305,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="2121761279"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -1316,6 +1364,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="1920122591"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
@@ -1369,6 +1418,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="2121761695"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -1384,6 +1434,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.31252887138665114"/>
+          <c:y val="0.17122743288652659"/>
+          <c:w val="0.36715637034214682"/>
+          <c:h val="5.1136733747729361E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2017,16 +2077,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>314324</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>152399</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>152399</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2350,184 +2410,267 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.5703125" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2">
+        <v>53</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1062530.19</v>
+      </c>
+      <c r="E2" s="2">
+        <v>754.59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1066000</v>
+      </c>
+      <c r="E3" s="2">
+        <v>756.49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1060000</v>
+      </c>
+      <c r="E4" s="2">
+        <v>757.14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1060000</v>
+      </c>
+      <c r="E5" s="2">
+        <v>757.14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="4">
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="4">
         <v>1060000</v>
       </c>
-      <c r="C2" s="2">
+      <c r="E6" s="2">
         <v>757.14</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="4">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="4">
         <v>1060000</v>
       </c>
-      <c r="C3" s="2">
+      <c r="E7" s="2">
         <v>757.14</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="4">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="4">
         <v>1060000</v>
       </c>
-      <c r="C4" s="2">
+      <c r="E8" s="2">
         <v>757.14</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="4">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="4">
         <v>1060000</v>
       </c>
-      <c r="C5" s="2">
+      <c r="E9" s="2">
         <v>757.14</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="4">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="4">
         <v>1060000</v>
       </c>
-      <c r="C6" s="2">
+      <c r="E10" s="2">
         <v>757.14</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="4">
-        <v>1060000</v>
-      </c>
-      <c r="C7" s="2">
-        <v>757.14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="4">
-        <v>1060000</v>
-      </c>
-      <c r="C8" s="2">
-        <v>757.14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="4">
-        <v>1066000</v>
-      </c>
-      <c r="C9" s="2">
-        <v>756.49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="4">
-        <v>1062530.19</v>
-      </c>
-      <c r="C10" s="2">
-        <v>754.59</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="4">
+        <v>34</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="4">
         <v>1084000</v>
       </c>
-      <c r="C11" s="2">
+      <c r="E11" s="2">
         <v>743.05</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="4">
+        <v>35</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="4">
         <v>1108000</v>
       </c>
-      <c r="C12" s="2">
+      <c r="E12" s="2">
         <v>728.95</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="4">
+        <v>36</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="4">
         <v>1108000</v>
       </c>
-      <c r="C13" s="2">
+      <c r="E13" s="2">
         <v>728.95</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="4">
+        <v>37</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="4">
         <v>1074100</v>
       </c>
-      <c r="C14" s="2">
+      <c r="E14" s="2">
         <v>695.28</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C15" s="2"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C16" s="2"/>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E16" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C14">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C14">
-      <sortCondition descending="1" ref="C1:C14"/>
+  <autoFilter ref="A1:E14" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E14">
+      <sortCondition descending="1" ref="E1:E14"/>
     </sortState>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A17:A23">
@@ -2539,19 +2682,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
     <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="29.28515625" bestFit="1" customWidth="1"/>
@@ -2971,12 +3114,32 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D16" s="2"/>
     </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:I14">
+  <autoFilter ref="A1:I14" xr:uid="{00000000-0009-0000-0000-000001000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I14">
       <sortCondition descending="1" ref="D1:D14"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>